<commit_message>
Tidy up the project code
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\RPA TAM\Source Code\RPA_PDCA\PDCA_7\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{652B66C0-0480-41BB-91D9-87D3BBCE6982}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E44E5994-5625-4A76-9497-0BC88F494FD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="85">
   <si>
     <t>Name</t>
   </si>
@@ -185,9 +185,6 @@
     <t>Query</t>
   </si>
   <si>
-    <t>CBU_Report_FileName</t>
-  </si>
-  <si>
     <t>Shipping Data TMC ETD &lt;BL date&gt;</t>
   </si>
   <si>
@@ -257,16 +254,31 @@
     <t>[RPA PDCA 7] Process Finished</t>
   </si>
   <si>
-    <t>Temp_Folder</t>
-  </si>
-  <si>
-    <t>E:\RPA_PDCA\PDCA_7\Data\Temp</t>
-  </si>
-  <si>
     <t>[RPA PDCA 7] Summary Report</t>
   </si>
   <si>
     <t>PDCA_7_Summary_Report_Subject</t>
+  </si>
+  <si>
+    <t>SendSummaryEmailTime</t>
+  </si>
+  <si>
+    <t>TLSCBUFile_Folder</t>
+  </si>
+  <si>
+    <t>E:\RPA_PDCA\PDCA_7\Data\TLSCBU</t>
+  </si>
+  <si>
+    <t>Summary_Folder</t>
+  </si>
+  <si>
+    <t>E:\RPA_PDCA\PDCA_7\Data\Summary</t>
+  </si>
+  <si>
+    <t>SummaryReport_FileName</t>
+  </si>
+  <si>
+    <t>Summary_Report.xlsx</t>
   </si>
 </sst>
 </file>
@@ -643,9 +655,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1001"/>
+  <dimension ref="A1:Z1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -696,7 +708,7 @@
         <v>46</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
@@ -717,7 +729,7 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>22</v>
@@ -751,18 +763,18 @@
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" t="s">
         <v>63</v>
-      </c>
-      <c r="B11" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" t="s">
         <v>65</v>
-      </c>
-      <c r="B12" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
@@ -770,89 +782,101 @@
         <v>52</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A14" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A15" s="2"/>
+      <c r="A15" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B16" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="14.25" customHeight="1">
       <c r="A17" s="2" t="s">
-        <v>58</v>
+        <v>79</v>
       </c>
       <c r="B17" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="14.25" customHeight="1">
       <c r="A18" s="2" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="B18" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A19" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B19" t="s">
-        <v>61</v>
-      </c>
-    </row>
+    <row r="19" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="20" spans="1:2" ht="14.25" customHeight="1">
       <c r="A20" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B20" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="21" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A21" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" t="s">
+        <v>53</v>
+      </c>
+    </row>
     <row r="22" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A22" t="s">
-        <v>68</v>
+      <c r="A22" s="2" t="s">
+        <v>83</v>
       </c>
       <c r="B22" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A23" t="s">
-        <v>75</v>
-      </c>
-      <c r="B23" t="s">
-        <v>76</v>
-      </c>
-    </row>
+    <row r="23" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="24" spans="1:2" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="B24" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="26" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A25" t="s">
+        <v>74</v>
+      </c>
+      <c r="B25" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A26" t="s">
+        <v>77</v>
+      </c>
+      <c r="B26" t="s">
+        <v>76</v>
+      </c>
+    </row>
     <row r="27" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="28" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A28" t="s">
+        <v>78</v>
+      </c>
+      <c r="B28">
+        <v>17</v>
+      </c>
+    </row>
     <row r="29" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="30" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="31" spans="1:2" ht="14.25" customHeight="1"/>
@@ -1826,6 +1850,8 @@
     <row r="999" ht="14.25" customHeight="1"/>
     <row r="1000" ht="14.25" customHeight="1"/>
     <row r="1001" ht="14.25" customHeight="1"/>
+    <row r="1002" ht="14.25" customHeight="1"/>
+    <row r="1003" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1837,7 +1863,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z989"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -3074,34 +3100,34 @@
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>